<commit_message>
update like & comment
</commit_message>
<xml_diff>
--- a/db/excel/sqlite-inovation-manager-ver-1.0.xlsx
+++ b/db/excel/sqlite-inovation-manager-ver-1.0.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14820" tabRatio="500" firstSheet="6" activeTab="12"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="tables" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="491">
   <si>
     <t>table_name</t>
   </si>
@@ -1509,6 +1509,9 @@
   </si>
   <si>
     <t>Động lực làm việc</t>
+  </si>
+  <si>
+    <t>default 0</t>
   </si>
 </sst>
 </file>
@@ -1939,9 +1942,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="160">
+  <cellStyleXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2438,7 +2443,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="160">
+  <cellStyles count="162">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2519,6 +2524,7 @@
     <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2598,6 +2604,7 @@
     <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3005,8 +3012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK217"/>
   <sheetViews>
-    <sheetView topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="B163" sqref="B163"/>
+    <sheetView tabSelected="1" topLeftCell="A150" workbookViewId="0">
+      <selection activeCell="C157" sqref="C157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -7208,7 +7215,9 @@
       <c r="D165" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="E165" s="6"/>
+      <c r="E165" s="6" t="s">
+        <v>490</v>
+      </c>
       <c r="F165" s="5"/>
       <c r="G165" s="6">
         <v>163</v>
@@ -7227,7 +7236,9 @@
       <c r="D166" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="E166" s="6"/>
+      <c r="E166" s="6" t="s">
+        <v>490</v>
+      </c>
       <c r="F166" s="5"/>
       <c r="G166" s="6">
         <v>164</v>
@@ -7246,7 +7257,9 @@
       <c r="D167" s="4" t="s">
         <v>444</v>
       </c>
-      <c r="E167" s="6"/>
+      <c r="E167" s="6" t="s">
+        <v>490</v>
+      </c>
       <c r="F167" s="5"/>
       <c r="G167" s="6">
         <v>165</v>
@@ -8582,7 +8595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
comment with file ok
</commit_message>
<xml_diff>
--- a/db/excel/sqlite-inovation-manager-ver-1.0.xlsx
+++ b/db/excel/sqlite-inovation-manager-ver-1.0.xlsx
@@ -1187,9 +1187,6 @@
     <t>đường dẫn liên kết file mở ra https://c3.mobifone.vn/file_/.....</t>
   </si>
   <si>
-    <t>đường dẫn file gốc đọc từ ổ cứng /upload.../</t>
-  </si>
-  <si>
     <t>Mã user thực hiện tạo file này</t>
   </si>
   <si>
@@ -1373,9 +1370,6 @@
     <t xml:space="preserve">, FOREIGN KEY (organization_id) REFERENCES organizations(id) , FOREIGN KEY (parent_id) REFERENCES ideas(id) , FOREIGN KEY (user_id) REFERENCES users(id) </t>
   </si>
   <si>
-    <t xml:space="preserve">,  FOREIGN KEY (user_id) REFERENCES users(id) </t>
-  </si>
-  <si>
     <t xml:space="preserve">,  FOREIGN KEY (organization_id) REFERENCES organizations(id) </t>
   </si>
   <si>
@@ -1518,6 +1512,12 @@
   </si>
   <si>
     <t>đối tượng json ghi các user nào đã voted cho ý tưởng này [1,2,3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">,   UNIQUE(file_path), FOREIGN KEY (user_id) REFERENCES users(id) </t>
+  </si>
+  <si>
+    <t>đường dẫn file gốc đọc từ ổ cứng là duy nhất cho mỗi file, đường dẫn tuyệt đối __dirname__...</t>
   </si>
 </sst>
 </file>
@@ -1948,9 +1948,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="166">
+  <cellStyleXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2453,7 +2455,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="166">
+  <cellStyles count="168">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2537,6 +2539,7 @@
     <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="163" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="165" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="167" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2619,6 +2622,7 @@
     <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="162" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="164" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="166" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3026,8 +3030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="C193" sqref="C193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="23" x14ac:dyDescent="0"/>
@@ -4094,7 +4098,7 @@
         <v>37</v>
       </c>
       <c r="D2" s="113" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="11" t="s">
@@ -4115,7 +4119,7 @@
         <v>38</v>
       </c>
       <c r="D3" s="113" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="11"/>
@@ -4134,7 +4138,7 @@
         <v>39</v>
       </c>
       <c r="D4" s="113" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E4" s="10"/>
       <c r="F4" s="11"/>
@@ -4153,7 +4157,7 @@
         <v>40</v>
       </c>
       <c r="D5" s="113" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="13"/>
@@ -4169,10 +4173,10 @@
         <v>4</v>
       </c>
       <c r="C6" s="91" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D6" s="113" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="13"/>
@@ -4191,7 +4195,7 @@
         <v>41</v>
       </c>
       <c r="D7" s="113" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="13"/>
@@ -4210,7 +4214,7 @@
         <v>42</v>
       </c>
       <c r="D8" s="114" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>43</v>
@@ -4231,10 +4235,10 @@
         <v>45</v>
       </c>
       <c r="D9" s="115" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F9" s="18"/>
       <c r="G9" s="6">
@@ -4252,7 +4256,7 @@
         <v>46</v>
       </c>
       <c r="D10" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E10" s="20"/>
       <c r="F10" s="6"/>
@@ -4271,7 +4275,7 @@
         <v>47</v>
       </c>
       <c r="D11" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="6"/>
@@ -4290,7 +4294,7 @@
         <v>49</v>
       </c>
       <c r="D12" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E12" s="20"/>
       <c r="F12" s="6"/>
@@ -4309,7 +4313,7 @@
         <v>51</v>
       </c>
       <c r="D13" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E13" s="20"/>
       <c r="F13" s="6"/>
@@ -4328,7 +4332,7 @@
         <v>52</v>
       </c>
       <c r="D14" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E14" s="20"/>
       <c r="F14" s="6"/>
@@ -4347,7 +4351,7 @@
         <v>53</v>
       </c>
       <c r="D15" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E15" s="20"/>
       <c r="F15" s="6"/>
@@ -4366,7 +4370,7 @@
         <v>54</v>
       </c>
       <c r="D16" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E16" s="20"/>
       <c r="F16" s="6"/>
@@ -4385,7 +4389,7 @@
         <v>55</v>
       </c>
       <c r="D17" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E17" s="20"/>
       <c r="F17" s="6"/>
@@ -4404,7 +4408,7 @@
         <v>57</v>
       </c>
       <c r="D18" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="6"/>
@@ -4423,7 +4427,7 @@
         <v>42</v>
       </c>
       <c r="D19" s="114" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="6"/>
@@ -4442,10 +4446,10 @@
         <v>58</v>
       </c>
       <c r="D20" s="117" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E20" s="24" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="F20" s="25"/>
       <c r="G20" s="6">
@@ -4463,10 +4467,10 @@
         <v>60</v>
       </c>
       <c r="D21" s="118" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F21" s="18"/>
       <c r="G21" s="6">
@@ -4484,7 +4488,7 @@
         <v>61</v>
       </c>
       <c r="D22" s="119" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E22" s="26"/>
       <c r="F22" s="6"/>
@@ -4503,7 +4507,7 @@
         <v>62</v>
       </c>
       <c r="D23" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E23" s="26"/>
       <c r="F23" s="6"/>
@@ -4522,7 +4526,7 @@
         <v>63</v>
       </c>
       <c r="D24" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E24" s="20"/>
       <c r="F24" s="6"/>
@@ -4541,7 +4545,7 @@
         <v>42</v>
       </c>
       <c r="D25" s="114" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E25" s="26"/>
       <c r="F25" s="6"/>
@@ -4554,13 +4558,13 @@
         <v>59</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C26" s="95" t="s">
         <v>65</v>
       </c>
       <c r="D26" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E26" s="26"/>
       <c r="F26" s="6"/>
@@ -4579,7 +4583,7 @@
         <v>67</v>
       </c>
       <c r="D27" s="119" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E27" s="26" t="s">
         <v>68</v>
@@ -4600,7 +4604,7 @@
         <v>70</v>
       </c>
       <c r="D28" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E28" s="26"/>
       <c r="F28" s="6"/>
@@ -4619,7 +4623,7 @@
         <v>72</v>
       </c>
       <c r="D29" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E29" s="26"/>
       <c r="F29" s="6"/>
@@ -4638,7 +4642,7 @@
         <v>73</v>
       </c>
       <c r="D30" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E30" s="26"/>
       <c r="F30" s="6"/>
@@ -4657,7 +4661,7 @@
         <v>75</v>
       </c>
       <c r="D31" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E31" s="26"/>
       <c r="F31" s="6"/>
@@ -4676,7 +4680,7 @@
         <v>76</v>
       </c>
       <c r="D32" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E32" s="26"/>
       <c r="F32" s="6"/>
@@ -4695,7 +4699,7 @@
         <v>77</v>
       </c>
       <c r="D33" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="6"/>
@@ -4714,7 +4718,7 @@
         <v>78</v>
       </c>
       <c r="D34" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="6"/>
@@ -4733,7 +4737,7 @@
         <v>79</v>
       </c>
       <c r="D35" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="6"/>
@@ -4752,7 +4756,7 @@
         <v>80</v>
       </c>
       <c r="D36" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="6"/>
@@ -4771,10 +4775,10 @@
         <v>81</v>
       </c>
       <c r="D37" s="117" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E37" s="24" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F37" s="25"/>
       <c r="G37" s="6">
@@ -4792,10 +4796,10 @@
         <v>83</v>
       </c>
       <c r="D38" s="118" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F38" s="18"/>
       <c r="G38" s="6">
@@ -4807,13 +4811,13 @@
         <v>82</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C39" s="93" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D39" s="118" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E39" s="17"/>
       <c r="F39" s="18"/>
@@ -4832,7 +4836,7 @@
         <v>85</v>
       </c>
       <c r="D40" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E40" s="26"/>
       <c r="F40" s="6"/>
@@ -4851,7 +4855,7 @@
         <v>86</v>
       </c>
       <c r="D41" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="6"/>
@@ -4870,7 +4874,7 @@
         <v>87</v>
       </c>
       <c r="D42" s="119" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="6"/>
@@ -4889,7 +4893,7 @@
         <v>77</v>
       </c>
       <c r="D43" s="119" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E43" s="20"/>
       <c r="F43" s="6"/>
@@ -4908,7 +4912,7 @@
         <v>78</v>
       </c>
       <c r="D44" s="119" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E44" s="20"/>
       <c r="F44" s="6"/>
@@ -4927,7 +4931,7 @@
         <v>42</v>
       </c>
       <c r="D45" s="114" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E45" s="20"/>
       <c r="F45" s="6"/>
@@ -4946,10 +4950,10 @@
         <v>88</v>
       </c>
       <c r="D46" s="117" t="s">
+        <v>439</v>
+      </c>
+      <c r="E46" s="24" t="s">
         <v>440</v>
-      </c>
-      <c r="E46" s="24" t="s">
-        <v>441</v>
       </c>
       <c r="F46" s="25"/>
       <c r="G46" s="6">
@@ -4967,10 +4971,10 @@
         <v>90</v>
       </c>
       <c r="D47" s="115" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F47" s="31"/>
       <c r="G47" s="6">
@@ -4988,7 +4992,7 @@
         <v>91</v>
       </c>
       <c r="D48" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E48" s="32"/>
       <c r="F48" s="33"/>
@@ -5007,7 +5011,7 @@
         <v>93</v>
       </c>
       <c r="D49" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E49" s="32"/>
       <c r="F49" s="33"/>
@@ -5026,7 +5030,7 @@
         <v>95</v>
       </c>
       <c r="D50" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E50" s="32"/>
       <c r="F50" s="33"/>
@@ -5045,7 +5049,7 @@
         <v>97</v>
       </c>
       <c r="D51" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E51" s="32"/>
       <c r="F51" s="33"/>
@@ -5064,7 +5068,7 @@
         <v>99</v>
       </c>
       <c r="D52" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E52" s="32"/>
       <c r="F52" s="33"/>
@@ -5083,7 +5087,7 @@
         <v>100</v>
       </c>
       <c r="D53" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E53" s="32"/>
       <c r="F53" s="33"/>
@@ -5102,7 +5106,7 @@
         <v>101</v>
       </c>
       <c r="D54" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E54" s="32"/>
       <c r="F54" s="33"/>
@@ -5121,7 +5125,7 @@
         <v>103</v>
       </c>
       <c r="D55" s="120" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E55" s="32"/>
       <c r="F55" s="33"/>
@@ -5140,7 +5144,7 @@
         <v>105</v>
       </c>
       <c r="D56" s="120" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E56" s="32"/>
       <c r="F56" s="33"/>
@@ -5159,7 +5163,7 @@
         <v>107</v>
       </c>
       <c r="D57" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E57" s="32"/>
       <c r="F57" s="33"/>
@@ -5178,7 +5182,7 @@
         <v>108</v>
       </c>
       <c r="D58" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E58" s="32"/>
       <c r="F58" s="33"/>
@@ -5197,7 +5201,7 @@
         <v>77</v>
       </c>
       <c r="D59" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E59" s="20"/>
       <c r="F59" s="6"/>
@@ -5216,7 +5220,7 @@
         <v>78</v>
       </c>
       <c r="D60" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E60" s="20"/>
       <c r="F60" s="6"/>
@@ -5235,7 +5239,7 @@
         <v>79</v>
       </c>
       <c r="D61" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E61" s="20"/>
       <c r="F61" s="6"/>
@@ -5254,7 +5258,7 @@
         <v>80</v>
       </c>
       <c r="D62" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="6"/>
@@ -5273,7 +5277,7 @@
         <v>42</v>
       </c>
       <c r="D63" s="114" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E63" s="32"/>
       <c r="F63" s="33"/>
@@ -5292,10 +5296,10 @@
         <v>110</v>
       </c>
       <c r="D64" s="117" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E64" s="37" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="F64" s="38"/>
       <c r="G64" s="6">
@@ -5304,16 +5308,16 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="109" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B65" s="28" t="s">
         <v>7</v>
       </c>
       <c r="C65" s="94" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D65" s="117" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E65" s="37"/>
       <c r="F65" s="25"/>
@@ -5323,16 +5327,16 @@
     </row>
     <row r="66" spans="1:7" ht="36">
       <c r="A66" s="109" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B66" s="28" t="s">
         <v>48</v>
       </c>
       <c r="C66" s="94" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D66" s="117" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E66" s="37"/>
       <c r="F66" s="25"/>
@@ -5342,16 +5346,16 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="109" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B67" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C67" s="94" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D67" s="117" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E67" s="37"/>
       <c r="F67" s="25"/>
@@ -5370,10 +5374,10 @@
         <v>112</v>
       </c>
       <c r="D68" s="115" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E68" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F68" s="31"/>
       <c r="G68" s="6">
@@ -5391,7 +5395,7 @@
         <v>114</v>
       </c>
       <c r="D69" s="121" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E69" s="39"/>
       <c r="F69" s="40"/>
@@ -5410,7 +5414,7 @@
         <v>116</v>
       </c>
       <c r="D70" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E70" s="39"/>
       <c r="F70" s="40"/>
@@ -5429,7 +5433,7 @@
         <v>358</v>
       </c>
       <c r="D71" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E71" s="42"/>
       <c r="F71" s="43"/>
@@ -5448,7 +5452,7 @@
         <v>119</v>
       </c>
       <c r="D72" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E72" s="42"/>
       <c r="F72" s="43"/>
@@ -5467,7 +5471,7 @@
         <v>121</v>
       </c>
       <c r="D73" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E73" s="42"/>
       <c r="F73" s="43"/>
@@ -5486,7 +5490,7 @@
         <v>123</v>
       </c>
       <c r="D74" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E74" s="39"/>
       <c r="F74" s="40"/>
@@ -5505,7 +5509,7 @@
         <v>125</v>
       </c>
       <c r="D75" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E75" s="39"/>
       <c r="F75" s="40"/>
@@ -5524,7 +5528,7 @@
         <v>127</v>
       </c>
       <c r="D76" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E76" s="39"/>
       <c r="F76" s="40"/>
@@ -5543,7 +5547,7 @@
         <v>129</v>
       </c>
       <c r="D77" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E77" s="39"/>
       <c r="F77" s="40" t="s">
@@ -5558,13 +5562,13 @@
         <v>111</v>
       </c>
       <c r="B78" s="41" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="C78" s="92" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="D78" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E78" s="39"/>
       <c r="F78" s="40"/>
@@ -5583,7 +5587,7 @@
         <v>355</v>
       </c>
       <c r="D79" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E79" s="39"/>
       <c r="F79" s="40"/>
@@ -5602,7 +5606,7 @@
         <v>356</v>
       </c>
       <c r="D80" s="121" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E80" s="39"/>
       <c r="F80" s="40"/>
@@ -5618,10 +5622,10 @@
         <v>132</v>
       </c>
       <c r="C81" s="92" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D81" s="122" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E81" s="39" t="s">
         <v>68</v>
@@ -5642,7 +5646,7 @@
         <v>133</v>
       </c>
       <c r="D82" s="122" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E82" s="39"/>
       <c r="F82" s="40"/>
@@ -5661,7 +5665,7 @@
         <v>135</v>
       </c>
       <c r="D83" s="122" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E83" s="39"/>
       <c r="F83" s="40"/>
@@ -5680,7 +5684,7 @@
         <v>137</v>
       </c>
       <c r="D84" s="121" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E84" s="20"/>
       <c r="F84" s="6"/>
@@ -5699,7 +5703,7 @@
         <v>139</v>
       </c>
       <c r="D85" s="121" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="6"/>
@@ -5718,7 +5722,7 @@
         <v>77</v>
       </c>
       <c r="D86" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="6"/>
@@ -5737,7 +5741,7 @@
         <v>78</v>
       </c>
       <c r="D87" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E87" s="20"/>
       <c r="F87" s="6"/>
@@ -5756,7 +5760,7 @@
         <v>354</v>
       </c>
       <c r="D88" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="6"/>
@@ -5775,7 +5779,7 @@
         <v>80</v>
       </c>
       <c r="D89" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E89" s="20"/>
       <c r="F89" s="6"/>
@@ -5794,7 +5798,7 @@
         <v>142</v>
       </c>
       <c r="D90" s="122" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E90" s="20"/>
       <c r="F90" s="6"/>
@@ -5813,7 +5817,7 @@
         <v>144</v>
       </c>
       <c r="D91" s="122" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E91" s="20"/>
       <c r="F91" s="6"/>
@@ -5832,10 +5836,10 @@
         <v>145</v>
       </c>
       <c r="D92" s="123" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E92" s="112" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="F92" s="25"/>
       <c r="G92" s="6">
@@ -5851,10 +5855,10 @@
       </c>
       <c r="C93" s="94"/>
       <c r="D93" s="115" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E93" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F93" s="25"/>
       <c r="G93" s="6">
@@ -5870,7 +5874,7 @@
       </c>
       <c r="C94" s="94"/>
       <c r="D94" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E94" s="37"/>
       <c r="F94" s="25"/>
@@ -5887,7 +5891,7 @@
       </c>
       <c r="C95" s="94"/>
       <c r="D95" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E95" s="37"/>
       <c r="F95" s="25"/>
@@ -5904,7 +5908,7 @@
       </c>
       <c r="C96" s="94"/>
       <c r="D96" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E96" s="37"/>
       <c r="F96" s="25"/>
@@ -5921,7 +5925,7 @@
       </c>
       <c r="C97" s="94"/>
       <c r="D97" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E97" s="37"/>
       <c r="F97" s="25"/>
@@ -5938,7 +5942,7 @@
       </c>
       <c r="C98" s="94"/>
       <c r="D98" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E98" s="37"/>
       <c r="F98" s="25"/>
@@ -5955,7 +5959,7 @@
       </c>
       <c r="C99" s="94"/>
       <c r="D99" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E99" s="37"/>
       <c r="F99" s="25"/>
@@ -5972,7 +5976,7 @@
       </c>
       <c r="C100" s="94"/>
       <c r="D100" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E100" s="37" t="s">
         <v>68</v>
@@ -5993,7 +5997,7 @@
         <v>149</v>
       </c>
       <c r="D101" s="124" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E101" s="46"/>
       <c r="F101" s="6"/>
@@ -6012,7 +6016,7 @@
         <v>150</v>
       </c>
       <c r="D102" s="124" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E102" s="46"/>
       <c r="F102" s="6"/>
@@ -6031,7 +6035,7 @@
         <v>152</v>
       </c>
       <c r="D103" s="124" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E103" s="46"/>
       <c r="F103" s="6"/>
@@ -6050,7 +6054,7 @@
         <v>153</v>
       </c>
       <c r="D104" s="124" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E104" s="46"/>
       <c r="F104" s="6"/>
@@ -6069,7 +6073,7 @@
         <v>77</v>
       </c>
       <c r="D105" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E105" s="20"/>
       <c r="F105" s="6"/>
@@ -6088,7 +6092,7 @@
         <v>78</v>
       </c>
       <c r="D106" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E106" s="20"/>
       <c r="F106" s="6"/>
@@ -6107,7 +6111,7 @@
         <v>79</v>
       </c>
       <c r="D107" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E107" s="20"/>
       <c r="F107" s="6"/>
@@ -6126,7 +6130,7 @@
         <v>80</v>
       </c>
       <c r="D108" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E108" s="20"/>
       <c r="F108" s="6"/>
@@ -6145,7 +6149,7 @@
         <v>154</v>
       </c>
       <c r="D109" s="117" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E109" s="47" t="s">
         <v>155</v>
@@ -6166,10 +6170,10 @@
         <v>157</v>
       </c>
       <c r="D110" s="115" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E110" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F110" s="18"/>
       <c r="G110" s="6">
@@ -6187,7 +6191,7 @@
         <v>158</v>
       </c>
       <c r="D111" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E111" s="20"/>
       <c r="F111" s="6"/>
@@ -6206,7 +6210,7 @@
         <v>159</v>
       </c>
       <c r="D112" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E112" s="20"/>
       <c r="F112" s="6"/>
@@ -6225,7 +6229,7 @@
         <v>160</v>
       </c>
       <c r="D113" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E113" s="20"/>
       <c r="F113" s="6"/>
@@ -6244,7 +6248,7 @@
         <v>95</v>
       </c>
       <c r="D114" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E114" s="20"/>
       <c r="F114" s="6"/>
@@ -6263,7 +6267,7 @@
         <v>97</v>
       </c>
       <c r="D115" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E115" s="20"/>
       <c r="F115" s="6"/>
@@ -6282,7 +6286,7 @@
         <v>99</v>
       </c>
       <c r="D116" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E116" s="20"/>
       <c r="F116" s="6"/>
@@ -6301,7 +6305,7 @@
         <v>161</v>
       </c>
       <c r="D117" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E117" s="20"/>
       <c r="F117" s="6"/>
@@ -6320,7 +6324,7 @@
         <v>162</v>
       </c>
       <c r="D118" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E118" s="20"/>
       <c r="F118" s="6"/>
@@ -6339,7 +6343,7 @@
         <v>163</v>
       </c>
       <c r="D119" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E119" s="20"/>
       <c r="F119" s="6"/>
@@ -6358,7 +6362,7 @@
         <v>164</v>
       </c>
       <c r="D120" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E120" s="20"/>
       <c r="F120" s="6"/>
@@ -6377,7 +6381,7 @@
         <v>165</v>
       </c>
       <c r="D121" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E121" s="20"/>
       <c r="F121" s="6"/>
@@ -6396,7 +6400,7 @@
         <v>77</v>
       </c>
       <c r="D122" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E122" s="20"/>
       <c r="F122" s="6"/>
@@ -6415,7 +6419,7 @@
         <v>78</v>
       </c>
       <c r="D123" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E123" s="20"/>
       <c r="F123" s="6"/>
@@ -6434,7 +6438,7 @@
         <v>79</v>
       </c>
       <c r="D124" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E124" s="20"/>
       <c r="F124" s="6"/>
@@ -6453,7 +6457,7 @@
         <v>80</v>
       </c>
       <c r="D125" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E125" s="20"/>
       <c r="F125" s="6"/>
@@ -6472,7 +6476,7 @@
         <v>42</v>
       </c>
       <c r="D126" s="114" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E126" s="20"/>
       <c r="F126" s="6"/>
@@ -6491,10 +6495,10 @@
         <v>166</v>
       </c>
       <c r="D127" s="117" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E127" s="24" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F127" s="25"/>
       <c r="G127" s="6">
@@ -6512,10 +6516,10 @@
         <v>168</v>
       </c>
       <c r="D128" s="118" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E128" s="51" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F128" s="18"/>
       <c r="G128" s="6">
@@ -6533,7 +6537,7 @@
         <v>170</v>
       </c>
       <c r="D129" s="125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E129" s="49"/>
       <c r="F129" s="13"/>
@@ -6552,7 +6556,7 @@
         <v>171</v>
       </c>
       <c r="D130" s="125" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E130" s="50"/>
       <c r="F130" s="13"/>
@@ -6571,7 +6575,7 @@
         <v>173</v>
       </c>
       <c r="D131" s="125" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E131" s="50"/>
       <c r="F131" s="13"/>
@@ -6590,7 +6594,7 @@
         <v>175</v>
       </c>
       <c r="D132" s="125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E132" s="50"/>
       <c r="F132" s="13"/>
@@ -6609,7 +6613,7 @@
         <v>176</v>
       </c>
       <c r="D133" s="125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E133" s="50"/>
       <c r="F133" s="13"/>
@@ -6628,7 +6632,7 @@
         <v>178</v>
       </c>
       <c r="D134" s="125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E134" s="50"/>
       <c r="F134" s="13"/>
@@ -6647,7 +6651,7 @@
         <v>180</v>
       </c>
       <c r="D135" s="125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E135" s="50"/>
       <c r="F135" s="13"/>
@@ -6666,7 +6670,7 @@
         <v>182</v>
       </c>
       <c r="D136" s="125" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E136" s="50"/>
       <c r="F136" s="13"/>
@@ -6685,7 +6689,7 @@
         <v>184</v>
       </c>
       <c r="D137" s="125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E137" s="50"/>
       <c r="F137" s="13"/>
@@ -6704,7 +6708,7 @@
         <v>186</v>
       </c>
       <c r="D138" s="125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E138" s="50"/>
       <c r="F138" s="13"/>
@@ -6723,7 +6727,7 @@
         <v>187</v>
       </c>
       <c r="D139" s="125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E139" s="50"/>
       <c r="F139" s="13"/>
@@ -6742,7 +6746,7 @@
         <v>188</v>
       </c>
       <c r="D140" s="125" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E140" s="50"/>
       <c r="F140" s="13"/>
@@ -6761,7 +6765,7 @@
         <v>77</v>
       </c>
       <c r="D141" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E141" s="20"/>
       <c r="F141" s="6"/>
@@ -6780,7 +6784,7 @@
         <v>78</v>
       </c>
       <c r="D142" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E142" s="20"/>
       <c r="F142" s="6"/>
@@ -6799,7 +6803,7 @@
         <v>79</v>
       </c>
       <c r="D143" s="116" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E143" s="20"/>
       <c r="F143" s="6"/>
@@ -6818,7 +6822,7 @@
         <v>80</v>
       </c>
       <c r="D144" s="116" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E144" s="20"/>
       <c r="F144" s="6"/>
@@ -6837,7 +6841,7 @@
         <v>190</v>
       </c>
       <c r="D145" s="125" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E145" s="50"/>
       <c r="F145" s="13"/>
@@ -6856,7 +6860,7 @@
         <v>42</v>
       </c>
       <c r="D146" s="114" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E146" s="50"/>
       <c r="F146" s="13"/>
@@ -6875,10 +6879,10 @@
         <v>191</v>
       </c>
       <c r="D147" s="117" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E147" s="24" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="F147" s="25"/>
       <c r="G147" s="6">
@@ -6896,10 +6900,10 @@
         <v>22</v>
       </c>
       <c r="D148" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E148" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F148" s="5"/>
       <c r="G148" s="6">
@@ -6914,10 +6918,10 @@
         <v>12</v>
       </c>
       <c r="C149" s="100" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D149" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E149" s="4"/>
       <c r="F149" s="5"/>
@@ -6933,10 +6937,10 @@
         <v>113</v>
       </c>
       <c r="C150" s="101" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E150" s="4"/>
       <c r="F150" s="5"/>
@@ -6949,13 +6953,13 @@
         <v>21</v>
       </c>
       <c r="B151" s="68" t="s">
+        <v>404</v>
+      </c>
+      <c r="C151" s="101" t="s">
         <v>405</v>
       </c>
-      <c r="C151" s="101" t="s">
-        <v>406</v>
-      </c>
       <c r="D151" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E151" s="4"/>
       <c r="F151" s="5"/>
@@ -6968,13 +6972,13 @@
         <v>21</v>
       </c>
       <c r="B152" s="68" t="s">
+        <v>402</v>
+      </c>
+      <c r="C152" s="101" t="s">
         <v>403</v>
       </c>
-      <c r="C152" s="101" t="s">
-        <v>404</v>
-      </c>
       <c r="D152" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E152" s="4"/>
       <c r="F152" s="5"/>
@@ -6993,7 +6997,7 @@
         <v>360</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E153" s="4"/>
       <c r="F153" s="5"/>
@@ -7012,7 +7016,7 @@
         <v>24</v>
       </c>
       <c r="D154" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E154" s="4"/>
       <c r="F154" s="5"/>
@@ -7031,7 +7035,7 @@
         <v>25</v>
       </c>
       <c r="D155" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E155" s="4"/>
       <c r="F155" s="5"/>
@@ -7050,7 +7054,7 @@
         <v>370</v>
       </c>
       <c r="D156" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E156" s="4"/>
       <c r="F156" s="5"/>
@@ -7069,7 +7073,7 @@
         <v>372</v>
       </c>
       <c r="D157" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E157" s="4"/>
       <c r="F157" s="5"/>
@@ -7088,7 +7092,7 @@
         <v>26</v>
       </c>
       <c r="D158" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E158" s="6"/>
       <c r="F158" s="5"/>
@@ -7107,7 +7111,7 @@
         <v>28</v>
       </c>
       <c r="D159" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E159" s="6"/>
       <c r="F159" s="5"/>
@@ -7126,7 +7130,7 @@
         <v>35</v>
       </c>
       <c r="D160" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E160" s="7"/>
       <c r="F160" s="8" t="s">
@@ -7147,7 +7151,7 @@
         <v>29</v>
       </c>
       <c r="D161" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E161" s="6"/>
       <c r="F161" s="5" t="s">
@@ -7162,13 +7166,13 @@
         <v>21</v>
       </c>
       <c r="B162" s="70" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="C162" s="92" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="D162" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E162" s="6"/>
       <c r="F162" s="5"/>
@@ -7187,7 +7191,7 @@
         <v>30</v>
       </c>
       <c r="D163" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E163" s="6"/>
       <c r="F163" s="5" t="s">
@@ -7205,10 +7209,10 @@
         <v>20</v>
       </c>
       <c r="C164" s="92" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="D164" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E164" s="6"/>
       <c r="F164" s="5"/>
@@ -7221,13 +7225,13 @@
         <v>21</v>
       </c>
       <c r="B165" s="67" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="C165" s="92" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D165" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E165" s="6"/>
       <c r="F165" s="5"/>
@@ -7246,10 +7250,10 @@
         <v>33</v>
       </c>
       <c r="D166" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E166" s="6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F166" s="5"/>
       <c r="G166" s="6">
@@ -7261,16 +7265,16 @@
         <v>21</v>
       </c>
       <c r="B167" s="67" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C167" s="92" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D167" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E167" s="6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F167" s="5"/>
       <c r="G167" s="6">
@@ -7282,16 +7286,16 @@
         <v>21</v>
       </c>
       <c r="B168" s="67" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C168" s="92" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D168" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E168" s="6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F168" s="5"/>
       <c r="G168" s="6">
@@ -7309,7 +7313,7 @@
         <v>34</v>
       </c>
       <c r="D169" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E169" s="6"/>
       <c r="F169" s="5"/>
@@ -7325,13 +7329,13 @@
         <v>14</v>
       </c>
       <c r="C170" s="92" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="D170" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E170" s="15" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="F170" s="5"/>
       <c r="G170" s="6">
@@ -7349,10 +7353,10 @@
         <v>349</v>
       </c>
       <c r="D171" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E171" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F171" s="6"/>
       <c r="G171" s="6">
@@ -7370,7 +7374,7 @@
         <v>359</v>
       </c>
       <c r="D172" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E172" s="17"/>
       <c r="F172" s="6"/>
@@ -7389,7 +7393,7 @@
         <v>353</v>
       </c>
       <c r="D173" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E173" s="6"/>
       <c r="F173" s="6"/>
@@ -7408,7 +7412,7 @@
         <v>373</v>
       </c>
       <c r="D174" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E174" s="6"/>
       <c r="F174" s="6"/>
@@ -7427,7 +7431,7 @@
         <v>372</v>
       </c>
       <c r="D175" s="4" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E175" s="4"/>
       <c r="F175" s="5"/>
@@ -7440,13 +7444,13 @@
         <v>348</v>
       </c>
       <c r="B176" s="71" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C176" s="92" t="s">
         <v>351</v>
       </c>
       <c r="D176" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E176" s="6"/>
       <c r="F176" s="6" t="s">
@@ -7467,7 +7471,7 @@
         <v>352</v>
       </c>
       <c r="D177" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E177" s="6"/>
       <c r="F177" s="6" t="s">
@@ -7488,10 +7492,10 @@
         <v>362</v>
       </c>
       <c r="D178" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E178" s="15" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="F178" s="6" t="s">
         <v>31</v>
@@ -7511,7 +7515,7 @@
         <v>366</v>
       </c>
       <c r="D179" s="126" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E179" s="6"/>
       <c r="F179" s="6" t="s">
@@ -7526,13 +7530,13 @@
         <v>363</v>
       </c>
       <c r="B180" s="73" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C180" s="102" t="s">
         <v>364</v>
       </c>
       <c r="D180" s="126" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E180" s="6"/>
       <c r="F180" s="6" t="s">
@@ -7553,7 +7557,7 @@
         <v>367</v>
       </c>
       <c r="D181" s="126" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E181" s="6"/>
       <c r="F181" s="6"/>
@@ -7572,10 +7576,10 @@
         <v>368</v>
       </c>
       <c r="D182" s="126" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E182" s="15" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F182" s="6"/>
       <c r="G182" s="6">
@@ -7584,7 +7588,7 @@
     </row>
     <row r="183" spans="1:7" ht="25">
       <c r="A183" s="88" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B183" s="74" t="s">
         <v>16</v>
@@ -7593,7 +7597,7 @@
         <v>366</v>
       </c>
       <c r="D183" s="127" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E183" s="53"/>
       <c r="F183" s="53" t="s">
@@ -7605,16 +7609,16 @@
     </row>
     <row r="184" spans="1:7" ht="25">
       <c r="A184" s="88" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B184" s="75" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="C184" s="103" t="s">
         <v>364</v>
       </c>
       <c r="D184" s="127" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E184" s="53"/>
       <c r="F184" s="53" t="s">
@@ -7626,7 +7630,7 @@
     </row>
     <row r="185" spans="1:7" ht="37">
       <c r="A185" s="88" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B185" s="74" t="s">
         <v>17</v>
@@ -7635,7 +7639,7 @@
         <v>367</v>
       </c>
       <c r="D185" s="127" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E185" s="53"/>
       <c r="F185" s="53"/>
@@ -7645,16 +7649,16 @@
     </row>
     <row r="186" spans="1:7" ht="25">
       <c r="A186" s="88" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B186" s="74" t="s">
         <v>350</v>
       </c>
       <c r="C186" s="103" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D186" s="127" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E186" s="53"/>
       <c r="F186" s="53"/>
@@ -7664,19 +7668,19 @@
     </row>
     <row r="187" spans="1:7" ht="44">
       <c r="A187" s="88" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B187" s="74" t="s">
         <v>365</v>
       </c>
       <c r="C187" s="103" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D187" s="127" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E187" s="54" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F187" s="53"/>
       <c r="G187" s="6">
@@ -7691,13 +7695,13 @@
         <v>7</v>
       </c>
       <c r="C188" s="104" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D188" s="128" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E188" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F188" s="6"/>
       <c r="G188" s="6">
@@ -7712,10 +7716,10 @@
         <v>374</v>
       </c>
       <c r="C189" s="92" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D189" s="129" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E189" s="6"/>
       <c r="F189" s="6"/>
@@ -7734,7 +7738,7 @@
         <v>375</v>
       </c>
       <c r="D190" s="128" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E190" s="6"/>
       <c r="F190" s="6"/>
@@ -7753,7 +7757,7 @@
         <v>376</v>
       </c>
       <c r="D191" s="128" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E191" s="6"/>
       <c r="F191" s="6"/>
@@ -7772,7 +7776,7 @@
         <v>381</v>
       </c>
       <c r="D192" s="129" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E192" s="6"/>
       <c r="F192" s="6"/>
@@ -7780,7 +7784,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="193" spans="1:7" ht="25">
+    <row r="193" spans="1:7" ht="37">
       <c r="A193" s="89" t="s">
         <v>369</v>
       </c>
@@ -7788,10 +7792,10 @@
         <v>380</v>
       </c>
       <c r="C193" s="92" t="s">
-        <v>382</v>
+        <v>492</v>
       </c>
       <c r="D193" s="129" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E193" s="6"/>
       <c r="F193" s="6"/>
@@ -7810,7 +7814,7 @@
         <v>367</v>
       </c>
       <c r="D194" s="126" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E194" s="6"/>
       <c r="F194" s="6"/>
@@ -7818,7 +7822,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="195" spans="1:7" ht="25">
+    <row r="195" spans="1:7" ht="30">
       <c r="A195" s="89" t="s">
         <v>369</v>
       </c>
@@ -7826,13 +7830,13 @@
         <v>16</v>
       </c>
       <c r="C195" s="92" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D195" s="4" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E195" s="15" t="s">
-        <v>444</v>
+        <v>491</v>
       </c>
       <c r="F195" s="6" t="s">
         <v>31</v>
@@ -7843,19 +7847,19 @@
     </row>
     <row r="196" spans="1:7" ht="25">
       <c r="A196" s="88" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B196" s="76" t="s">
         <v>7</v>
       </c>
       <c r="C196" s="92" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D196" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E196" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F196" s="6"/>
       <c r="G196" s="6">
@@ -7864,16 +7868,16 @@
     </row>
     <row r="197" spans="1:7" ht="37">
       <c r="A197" s="88" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B197" s="76" t="s">
         <v>12</v>
       </c>
       <c r="C197" s="92" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D197" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E197" s="6"/>
       <c r="F197" s="6"/>
@@ -7883,16 +7887,16 @@
     </row>
     <row r="198" spans="1:7" ht="25">
       <c r="A198" s="88" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B198" s="74" t="s">
         <v>113</v>
       </c>
       <c r="C198" s="103" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D198" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E198" s="6"/>
       <c r="F198" s="6"/>
@@ -7902,16 +7906,16 @@
     </row>
     <row r="199" spans="1:7" ht="25">
       <c r="A199" s="88" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B199" s="76" t="s">
         <v>48</v>
       </c>
       <c r="C199" s="92" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D199" s="130" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E199" s="6"/>
       <c r="F199" s="6"/>
@@ -7921,16 +7925,16 @@
     </row>
     <row r="200" spans="1:7" ht="25">
       <c r="A200" s="88" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B200" s="76" t="s">
+        <v>395</v>
+      </c>
+      <c r="C200" s="92" t="s">
         <v>396</v>
       </c>
-      <c r="C200" s="92" t="s">
-        <v>397</v>
-      </c>
       <c r="D200" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E200" s="6"/>
       <c r="F200" s="6"/>
@@ -7940,16 +7944,16 @@
     </row>
     <row r="201" spans="1:7" ht="37">
       <c r="A201" s="88" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B201" s="76" t="s">
+        <v>397</v>
+      </c>
+      <c r="C201" s="92" t="s">
         <v>398</v>
       </c>
-      <c r="C201" s="92" t="s">
-        <v>399</v>
-      </c>
       <c r="D201" s="130" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E201" s="6"/>
       <c r="F201" s="6"/>
@@ -7959,16 +7963,16 @@
     </row>
     <row r="202" spans="1:7" ht="25">
       <c r="A202" s="88" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B202" s="76" t="s">
         <v>2</v>
       </c>
       <c r="C202" s="92" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D202" s="130" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F202" s="6"/>
       <c r="G202" s="6">
@@ -7977,16 +7981,16 @@
     </row>
     <row r="203" spans="1:7" ht="25">
       <c r="A203" s="88" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B203" s="76" t="s">
         <v>6</v>
       </c>
       <c r="C203" s="92" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D203" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F203" s="6"/>
       <c r="G203" s="6">
@@ -7995,19 +7999,19 @@
     </row>
     <row r="204" spans="1:7" ht="30">
       <c r="A204" s="137" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B204" s="133" t="s">
         <v>14</v>
       </c>
       <c r="C204" s="134" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D204" s="135" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E204" s="136" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F204" s="6"/>
       <c r="G204" s="6">
@@ -8016,19 +8020,19 @@
     </row>
     <row r="205" spans="1:7">
       <c r="A205" s="108" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B205" s="67" t="s">
         <v>7</v>
       </c>
       <c r="C205" s="92" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D205" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E205" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F205" s="6"/>
       <c r="G205" s="6">
@@ -8037,16 +8041,16 @@
     </row>
     <row r="206" spans="1:7">
       <c r="A206" s="108" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B206" s="74" t="s">
         <v>113</v>
       </c>
       <c r="C206" s="103" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D206" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="G206" s="6">
         <v>211</v>
@@ -8054,16 +8058,16 @@
     </row>
     <row r="207" spans="1:7">
       <c r="A207" s="108" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B207" s="67" t="s">
         <v>48</v>
       </c>
       <c r="C207" s="92" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D207" s="130" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E207" s="6"/>
       <c r="F207" s="6"/>
@@ -8073,16 +8077,16 @@
     </row>
     <row r="208" spans="1:7">
       <c r="A208" s="108" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B208" s="67" t="s">
         <v>2</v>
       </c>
       <c r="C208" s="92" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D208" s="130" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E208" s="6"/>
       <c r="F208" s="6"/>
@@ -8092,16 +8096,16 @@
     </row>
     <row r="209" spans="1:7">
       <c r="A209" s="108" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B209" s="67" t="s">
         <v>6</v>
       </c>
       <c r="C209" s="92" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D209" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E209" s="6"/>
       <c r="F209" s="6"/>
@@ -8111,16 +8115,16 @@
     </row>
     <row r="210" spans="1:7">
       <c r="A210" s="108" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B210" s="67" t="s">
         <v>14</v>
       </c>
       <c r="C210" s="92" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D210" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E210" s="6"/>
       <c r="F210" s="6"/>
@@ -8130,19 +8134,19 @@
     </row>
     <row r="211" spans="1:7">
       <c r="A211" s="107" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B211" s="67" t="s">
         <v>7</v>
       </c>
       <c r="C211" s="92" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="D211" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E211" s="17" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="F211" s="6"/>
       <c r="G211" s="6">
@@ -8151,16 +8155,16 @@
     </row>
     <row r="212" spans="1:7">
       <c r="A212" s="107" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B212" s="74" t="s">
         <v>113</v>
       </c>
       <c r="C212" s="103" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D212" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E212" s="6"/>
       <c r="F212" s="6"/>
@@ -8170,16 +8174,16 @@
     </row>
     <row r="213" spans="1:7" ht="91">
       <c r="A213" s="107" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B213" s="67" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C213" s="92" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D213" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E213" s="6"/>
       <c r="F213" s="6"/>
@@ -8189,16 +8193,16 @@
     </row>
     <row r="214" spans="1:7">
       <c r="A214" s="107" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B214" s="67" t="s">
         <v>48</v>
       </c>
       <c r="C214" s="92" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D214" s="130" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="E214" s="6"/>
       <c r="F214" s="6"/>
@@ -8208,16 +8212,16 @@
     </row>
     <row r="215" spans="1:7">
       <c r="A215" s="107" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B215" s="76" t="s">
+        <v>395</v>
+      </c>
+      <c r="C215" s="92" t="s">
         <v>396</v>
       </c>
-      <c r="C215" s="92" t="s">
-        <v>397</v>
-      </c>
       <c r="D215" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E215" s="6"/>
       <c r="F215" s="6"/>
@@ -8227,16 +8231,16 @@
     </row>
     <row r="216" spans="1:7" ht="36" customHeight="1">
       <c r="A216" s="107" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B216" s="67" t="s">
         <v>2</v>
       </c>
       <c r="C216" s="92" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D216" s="130" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="F216" s="6"/>
       <c r="G216" s="6">
@@ -8245,16 +8249,16 @@
     </row>
     <row r="217" spans="1:7" ht="36" customHeight="1">
       <c r="A217" s="107" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B217" s="67" t="s">
         <v>6</v>
       </c>
       <c r="C217" s="92" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="D217" s="130" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="F217" s="6"/>
       <c r="G217" s="6">
@@ -8263,19 +8267,19 @@
     </row>
     <row r="218" spans="1:7" ht="55" customHeight="1">
       <c r="A218" s="132" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B218" s="133" t="s">
         <v>14</v>
       </c>
       <c r="C218" s="134" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D218" s="135" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="E218" s="136" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F218" s="6"/>
       <c r="G218" s="6">
@@ -8324,10 +8328,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -8335,10 +8339,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -8346,10 +8350,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C4" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -8357,10 +8361,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -8368,10 +8372,10 @@
         <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -8379,10 +8383,10 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C7" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>
@@ -8559,10 +8563,10 @@
         <v>113</v>
       </c>
       <c r="D1" s="68" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E1" s="68" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="F1" s="67" t="s">
         <v>23</v>
@@ -8601,10 +8605,10 @@
         <v>19</v>
       </c>
       <c r="R1" s="67" t="s">
+        <v>387</v>
+      </c>
+      <c r="S1" s="67" t="s">
         <v>388</v>
-      </c>
-      <c r="S1" s="67" t="s">
-        <v>389</v>
       </c>
       <c r="T1" s="67" t="s">
         <v>32</v>
@@ -8657,10 +8661,10 @@
         <v>48</v>
       </c>
       <c r="E1" s="76" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F1" s="76" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G1" s="76" t="s">
         <v>2</v>
@@ -8681,7 +8685,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -8700,7 +8704,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="E3" s="6">
         <v>1</v>
@@ -8721,7 +8725,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -8740,7 +8744,7 @@
         <v>3</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -8759,7 +8763,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -8778,7 +8782,7 @@
         <v>3</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -8797,7 +8801,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -8816,7 +8820,7 @@
         <v>3</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -8914,13 +8918,13 @@
         <v>113</v>
       </c>
       <c r="C1" s="67" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D1" s="67" t="s">
         <v>48</v>
       </c>
       <c r="E1" s="76" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F1" s="67" t="s">
         <v>2</v>
@@ -8941,11 +8945,11 @@
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G2" s="6">
         <v>99</v>
@@ -8961,13 +8965,13 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="E3" s="6">
         <v>1</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
@@ -8983,11 +8987,11 @@
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G4" s="6">
         <v>2</v>
@@ -9003,11 +9007,11 @@
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G5" s="6">
         <v>3</v>
@@ -9023,11 +9027,11 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="G6" s="6">
         <v>4</v>
@@ -9043,11 +9047,11 @@
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G7" s="6">
         <v>5</v>
@@ -9236,7 +9240,7 @@
         <v>7</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C1" s="29" t="s">
         <v>84</v>
@@ -10365,10 +10369,10 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="3" spans="1:18">
@@ -10379,10 +10383,10 @@
         <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="H3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>